<commit_message>
Stable version: working backend/frontend with bug fixes
</commit_message>
<xml_diff>
--- a/server/All_Patients.xlsx
+++ b/server/All_Patients.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>sarasch25</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Suzanne</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Ismail</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-07-09</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Lumpectomy</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v>Anxiety</v>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v>suzaism25</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>